<commit_message>
Updated Data-Analysis_Ardientes.xlsx with new version
</commit_message>
<xml_diff>
--- a/Lab-20250913/Data-Analysis_Ardientes.xlsx
+++ b/Lab-20250913/Data-Analysis_Ardientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dardi\fba_it31s1\Lab-20250913\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC3F616-E8F6-4E54-8572-8F2ADDBF4540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2461AF86-3365-4792-9555-F7CEB393DECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{EE0BAA00-461C-478B-B827-BEAB6EE22138}"/>
+    <workbookView xWindow="5388" yWindow="2100" windowWidth="12492" windowHeight="8880" xr2:uid="{EE0BAA00-461C-478B-B827-BEAB6EE22138}"/>
   </bookViews>
   <sheets>
     <sheet name="VIEW" sheetId="1" r:id="rId1"/>
@@ -195,10 +195,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -7757,16 +7757,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Comparing the initial and Final summaries of data, it was clear that the final summary of data shows more organization, clarity, and data integrity. This is because it has gone through data clean-up in the phase of the CRISP-DM framework, which is the process where data is analyzed thoroughly by fixing naming, </a:t>
+            <a:t>Comparing the initial and Final summaries of data, it was clear that the final summary of data shows more organization, clarity, and data integrity. This is because it has gone through data clean-up in the phase of the CRISP-DM framework, which is the process where data is analyzed thoroughly by fixing naming, cleaning</a:t>
           </a:r>
-          <a:endParaRPr lang="en-PH" sz="2400" b="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-PH" sz="2400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> up redundancy and merging data that are in the same group.</a:t>
+          </a:r>
           <a:br>
             <a:rPr lang="en-PH" sz="2400">
               <a:solidFill>
@@ -8086,37 +8090,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88417B88-5DD8-4890-84BB-08B0FBA2320E}">
   <dimension ref="H9:AL26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I33" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AG76" sqref="AG76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="9" spans="8:38">
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="3"/>
       <c r="K9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="L9" s="4"/>
-      <c r="N9" s="2" t="s">
+      <c r="N9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="Q9" s="2" t="s">
+      <c r="O9" s="3"/>
+      <c r="Q9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="2"/>
+      <c r="R9" s="3"/>
       <c r="AB9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="AC9" s="1"/>
-      <c r="AE9" s="3" t="s">
+      <c r="AE9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AF9" s="3"/>
+      <c r="AF9" s="2"/>
       <c r="AH9" s="1" t="s">
         <v>34</v>
       </c>
@@ -8539,7 +8543,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62241C52-E675-4003-A4E5-E1A316DE4087}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635FF216-CADA-48B2-A472-69BDC3B2C198}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
   </ds:schemaRefs>

</xml_diff>